<commit_message>
Update PowerShell scripts used to create teams
</commit_message>
<xml_diff>
--- a/Files/Teams.xlsx
+++ b/Files/Teams.xlsx
@@ -30,9 +30,6 @@
     <t>Members</t>
   </si>
   <si>
-    <t>Team 1</t>
-  </si>
-  <si>
     <t>admin@cand3.onmicrosoft.com</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>katiej@cand3.onmicrosoft.com;rong@cand3.onmicrosoft.com</t>
   </si>
   <si>
-    <t>Team 2</t>
-  </si>
-  <si>
     <t>AccessType</t>
   </si>
   <si>
@@ -54,7 +48,13 @@
     <t>Public</t>
   </si>
   <si>
-    <t>Team 3</t>
+    <t>Team 51</t>
+  </si>
+  <si>
+    <t>Team 52</t>
+  </si>
+  <si>
+    <t>Team 53</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -412,30 +412,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -443,10 +443,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check in new changes
</commit_message>
<xml_diff>
--- a/Files/Teams.xlsx
+++ b/Files/Teams.xlsx
@@ -30,6 +30,9 @@
     <t>Members</t>
   </si>
   <si>
+    <t>Team 1</t>
+  </si>
+  <si>
     <t>admin@cand3.onmicrosoft.com</t>
   </si>
   <si>
@@ -39,6 +42,9 @@
     <t>katiej@cand3.onmicrosoft.com;rong@cand3.onmicrosoft.com</t>
   </si>
   <si>
+    <t>Team 2</t>
+  </si>
+  <si>
     <t>AccessType</t>
   </si>
   <si>
@@ -48,13 +54,7 @@
     <t>Public</t>
   </si>
   <si>
-    <t>Team 51</t>
-  </si>
-  <si>
-    <t>Team 52</t>
-  </si>
-  <si>
-    <t>Team 53</t>
+    <t>Team 3</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -412,30 +412,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -443,10 +443,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>